<commit_message>
ER atualizado e tabelas mapeadas na pasta 'tabelas novas'
</commit_message>
<xml_diff>
--- a/tabelas novas/1. user.xlsx
+++ b/tabelas novas/1. user.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\project123\tabelas novas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documentos\GitHub\project123\tabelas novas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="3888450FC4F50283A862C6CC171D4E856EB5F643" xr6:coauthVersionLast="10" xr6:coauthVersionMax="10" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4452"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Tabela Nome Antigo</t>
   </si>
@@ -167,13 +166,22 @@
   </si>
   <si>
     <t>post_graduation_id</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>profile_id</t>
+  </si>
+  <si>
+    <t>platoon_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +221,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -226,13 +246,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,20 +558,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -558,7 +580,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -567,7 +589,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,7 +598,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -585,7 +607,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -594,7 +616,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -603,7 +625,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -612,7 +634,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -621,7 +643,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -630,7 +652,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -639,7 +661,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -648,7 +670,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -657,7 +679,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -666,7 +688,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -675,7 +697,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -684,7 +706,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -693,7 +715,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -702,7 +724,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -711,7 +733,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -720,16 +742,15 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -738,7 +759,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -747,7 +768,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -756,7 +777,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -765,7 +786,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -774,7 +795,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -783,7 +804,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -792,7 +813,7 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -801,7 +822,7 @@
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -810,7 +831,7 @@
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -819,16 +840,15 @@
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -837,7 +857,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -845,6 +865,22 @@
         <v>48</v>
       </c>
       <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>